<commit_message>
User_defined_constraint as an alternative to unit_incremental_heat_rate
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/variable_efficiency.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/variable_efficiency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{7E25F1DF-6010-4BCD-8984-B89AB0F447D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{099E542F-2860-408A-8976-245006A32973}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{7E25F1DF-6010-4BCD-8984-B89AB0F447D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{906BAD32-BA62-4E72-873D-73039C6E64C2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6F728511-B5BA-484C-BEF6-08D3CC388B55}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>relationship_class:</t>
   </si>
   <si>
-    <t>unit__node__node</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
@@ -62,13 +59,16 @@
     <t>parameter name</t>
   </si>
   <si>
-    <t>unit_incremental_heat_rate</t>
-  </si>
-  <si>
     <t>operating_points</t>
   </si>
   <si>
     <t>unit__from_node</t>
+  </si>
+  <si>
+    <t>unit_flow_coefficient</t>
+  </si>
+  <si>
+    <t>unit__from_node__user_constraint</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -451,51 +451,51 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -503,8 +503,7 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <f>1/0.75</f>
-        <v>1.3333333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="C6">
         <v>0.4</v>
@@ -515,8 +514,7 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <f>1/0.7</f>
-        <v>1.4285714285714286</v>
+        <v>0.7</v>
       </c>
       <c r="C7">
         <v>0.7</v>
@@ -527,8 +525,7 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <f>1/0.667</f>
-        <v>1.4992503748125936</v>
+        <v>0.65</v>
       </c>
       <c r="C8">
         <v>1</v>

</xml_diff>